<commit_message>
starting on pitching stats
</commit_message>
<xml_diff>
--- a/csv/rosters.xlsx
+++ b/csv/rosters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1500" windowWidth="11700" windowHeight="13520" tabRatio="548" activeTab="1"/>
+    <workbookView xWindow="11500" yWindow="0" windowWidth="11700" windowHeight="13520" tabRatio="548"/>
   </bookViews>
   <sheets>
     <sheet name="whitesox" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="67">
   <si>
     <t>Luis Avilan</t>
   </si>
@@ -106,9 +106,6 @@
     <t>position</t>
   </si>
   <si>
-    <t>pitcher</t>
-  </si>
-  <si>
     <t>posnum</t>
   </si>
   <si>
@@ -215,13 +212,22 @@
   </si>
   <si>
     <t>Efren Navarro</t>
+  </si>
+  <si>
+    <t>Gregory Infante</t>
+  </si>
+  <si>
+    <t>Juan Minaya</t>
+  </si>
+  <si>
+    <t>Starting Pitcher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -241,6 +247,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -268,7 +281,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -276,6 +289,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -609,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -627,7 +642,7 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
@@ -641,7 +656,7 @@
         <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -652,7 +667,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -663,7 +678,7 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -674,7 +689,7 @@
         <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -685,7 +700,7 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -696,7 +711,7 @@
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -707,7 +722,7 @@
         <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -718,7 +733,7 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -729,7 +744,7 @@
         <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -740,7 +755,7 @@
         <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -751,7 +766,7 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -762,7 +777,7 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -773,114 +788,114 @@
         <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>13</v>
+      <c r="A15" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="B15" s="2">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" t="s">
-        <v>14</v>
+      <c r="A16" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="B16" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2">
-        <v>79</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" s="2">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>19</v>
       </c>
       <c r="B22" s="2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="2">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="B24" s="2">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C24" t="s">
         <v>21</v>
@@ -888,10 +903,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="2">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
         <v>21</v>
@@ -899,13 +914,35 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="2">
+        <v>26</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B28" s="2">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
-        <v>34</v>
+      <c r="C28" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -923,8 +960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -939,202 +976,202 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>36</v>
+      <c r="A2" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B2" s="2">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>37</v>
+      <c r="A3" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="B3" s="2">
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>38</v>
+      <c r="A4" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B4" s="2">
         <v>41</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>39</v>
+      <c r="A5" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B5" s="2">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>40</v>
+      <c r="A6" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="2">
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" t="s">
-        <v>41</v>
+      <c r="A7" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>42</v>
+      <c r="A8" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B8" s="2">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>43</v>
+      <c r="A9" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B9" s="2">
         <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>44</v>
+      <c r="A10" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B10" s="2">
         <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3">
-      <c r="A11" t="s">
-        <v>45</v>
+      <c r="A11" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="B11" s="2">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>46</v>
+      <c r="A12" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B12" s="2">
         <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>47</v>
+      <c r="A13" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="B13" s="2">
         <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>48</v>
+      <c r="A14" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="2">
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2">
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2">
         <v>2</v>
@@ -1145,18 +1182,18 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2">
         <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2">
         <v>18</v>
@@ -1167,18 +1204,18 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B22" s="2">
         <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="2">
         <v>5</v>
@@ -1189,7 +1226,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2">
         <v>8</v>
@@ -1200,7 +1237,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="2">
         <v>22</v>
@@ -1211,7 +1248,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="2">
         <v>12</v>
@@ -1222,13 +1259,13 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B27" s="2">
         <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>